<commit_message>
added mirror of a tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -322,7 +322,7 @@
     <t>Find first and last positions of an element in a sorted array</t>
   </si>
   <si>
-    <t>Find a Fixed Point (Value equal to index) in a given array</t>
+    <t>smallestEqual</t>
   </si>
   <si>
     <t>Search in a rotated sorted array</t>
@@ -1868,12 +1868,12 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="24.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="23.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1884,14 +1884,14 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1"/>
       <c r="B5" s="4"/>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="24.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="23.25">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="24.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="23.25">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="24.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="23.25">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="24.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="23.25">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="24.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="23.25">
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="24.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="23.25">
       <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="24.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="23.25">
       <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="24.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="23.25">
       <c r="A13" s="7" t="s">
         <v>6</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="24.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="23.25">
       <c r="A14" s="7" t="s">
         <v>6</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="24.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="23.25">
       <c r="A15" s="7" t="s">
         <v>6</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="24.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="23.25">
       <c r="A16" s="7" t="s">
         <v>6</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="24.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="23.25">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>101</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="17.25">
@@ -2948,7 +2948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="24">
       <c r="A105" s="7" t="s">
         <v>100</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="24">
       <c r="A106" s="7" t="s">
         <v>100</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="24">
       <c r="A107" s="7" t="s">
         <v>100</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="24">
       <c r="A108" s="7" t="s">
         <v>100</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="24">
       <c r="A109" s="7" t="s">
         <v>100</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="24">
       <c r="A110" s="7" t="s">
         <v>100</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="24">
       <c r="A111" s="7" t="s">
         <v>100</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="24">
       <c r="A112" s="7" t="s">
         <v>100</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="24">
       <c r="A113" s="7" t="s">
         <v>100</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="24">
       <c r="A114" s="7" t="s">
         <v>100</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="24">
       <c r="A115" s="7" t="s">
         <v>100</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="24">
       <c r="A116" s="7" t="s">
         <v>100</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="24">
       <c r="A117" s="7" t="s">
         <v>100</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="24">
       <c r="A118" s="7" t="s">
         <v>100</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="24">
       <c r="A119" s="7" t="s">
         <v>100</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="24">
       <c r="A120" s="7" t="s">
         <v>100</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="24">
       <c r="A121" s="7" t="s">
         <v>100</v>
       </c>

</xml_diff>